<commit_message>
May 12, 2025 update
</commit_message>
<xml_diff>
--- a/xlsxPCES/examples/euds.xlsx
+++ b/xlsxPCES/examples/euds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicol/Dropbox/github-repos/pcesapps-working/euds/xlsx/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicol/Dropbox/github-repos/pcesapps/euds/xlsx/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CF65F7-A63E-3C49-BC5B-47D1C1C0AD81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82691AA5-568F-8748-A0DE-A7B8E0DF7B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="980" windowWidth="34260" windowHeight="19580" activeTab="1" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
+    <workbookView xWindow="4220" yWindow="1480" windowWidth="25800" windowHeight="16620" activeTab="5" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="topo" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="192">
   <si>
     <t>Networks</t>
   </si>
@@ -190,12 +190,6 @@
     <t>exec time</t>
   </si>
   <si>
-    <t>const</t>
-  </si>
-  <si>
-    <t>perbyte</t>
-  </si>
-  <si>
     <t>CPU Entries</t>
   </si>
   <si>
@@ -346,9 +340,6 @@
     <t>generate</t>
   </si>
   <si>
-    <t>authenticate</t>
-  </si>
-  <si>
     <t>decrypt</t>
   </si>
   <si>
@@ -370,9 +361,6 @@
     <t>encrypt-AES-256-CBC</t>
   </si>
   <si>
-    <t>AMD EPYC 9534 64-Core Processor</t>
-  </si>
-  <si>
     <t>decrypt-AES-256-CBC</t>
   </si>
   <si>
@@ -385,21 +373,12 @@
     <t>decrypt-AES-128-CBC</t>
   </si>
   <si>
-    <t>Aruba 3810m</t>
-  </si>
-  <si>
     <t>switch</t>
   </si>
   <si>
     <t>Netgear GS324T</t>
   </si>
   <si>
-    <t>Netgear GS724T</t>
-  </si>
-  <si>
-    <t>Netgear GJS524e</t>
-  </si>
-  <si>
     <t>packet-return</t>
   </si>
   <si>
@@ -427,9 +406,6 @@
     <t>label</t>
   </si>
   <si>
-    <t>bypass</t>
-  </si>
-  <si>
     <t>srvcp</t>
   </si>
   <si>
@@ -511,12 +487,6 @@
     <t>$crypto,cp</t>
   </si>
   <si>
-    <t>encrypt-$crypto</t>
-  </si>
-  <si>
-    <t>decrypt-$crypto</t>
-  </si>
-  <si>
     <t>exp-5</t>
   </si>
   <si>
@@ -556,9 +526,6 @@
     <t>transfer</t>
   </si>
   <si>
-    <t>$pcktlen</t>
-  </si>
-  <si>
     <t>pvtNet</t>
   </si>
   <si>
@@ -583,9 +550,6 @@
     <t>pvtRtr</t>
   </si>
   <si>
-    <t>Cisco</t>
-  </si>
-  <si>
     <t>route</t>
   </si>
   <si>
@@ -610,29 +574,53 @@
     <t>$lambda,cp</t>
   </si>
   <si>
-    <t>$lambda</t>
-  </si>
-  <si>
-    <t>packet-process-0</t>
-  </si>
-  <si>
-    <t>packet-process-1</t>
-  </si>
-  <si>
-    <t>packet-process-2</t>
-  </si>
-  <si>
-    <t>packet-process-3</t>
-  </si>
-  <si>
     <t>euds_measure</t>
+  </si>
+  <si>
+    <t>float($lambda)</t>
+  </si>
+  <si>
+    <t>int($pcktlen)</t>
+  </si>
+  <si>
+    <t>encrypt-str($crypto)</t>
+  </si>
+  <si>
+    <t>decrypt-str($crypto)</t>
+  </si>
+  <si>
+    <t>Intel(R) Core(TM) i7-8650U CPU</t>
+  </si>
+  <si>
+    <t>AMD EPYC 7763 64-Core Processor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cisco 4300 </t>
+  </si>
+  <si>
+    <t>Netgear GJS524E</t>
+  </si>
+  <si>
+    <t>bandwidth</t>
+  </si>
+  <si>
+    <t>Aruba 3810</t>
+  </si>
+  <si>
+    <t>packet-process</t>
+  </si>
+  <si>
+    <t>hub</t>
+  </si>
+  <si>
+    <t>interruptdelay (musec)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -779,6 +767,13 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="40">
@@ -1205,7 +1200,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1218,6 +1213,11 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1595,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95325CDA-052A-9A47-A8FD-348C19C2091E}">
   <dimension ref="A2:H62"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView topLeftCell="A27" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1618,7 +1618,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -1632,74 +1632,74 @@
       <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="E4" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="F4" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="F5" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="F7" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1709,7 +1709,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -1726,17 +1726,17 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>117</v>
+        <v>163</v>
+      </c>
+      <c r="B14" t="s">
+        <v>112</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1744,7 +1744,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1755,17 +1755,17 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>117</v>
+        <v>166</v>
+      </c>
+      <c r="B17" t="s">
+        <v>186</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1773,7 +1773,7 @@
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1781,7 +1781,7 @@
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1789,7 +1789,7 @@
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1797,7 +1797,7 @@
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1818,7 +1818,7 @@
       <c r="B24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="4" t="s">
@@ -1830,43 +1830,43 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B25" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D25" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="E25" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D28" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="E28" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E29" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1876,7 +1876,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>9</v>
@@ -1884,7 +1884,7 @@
       <c r="C32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="5" t="s">
@@ -1902,10 +1902,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B33" t="s">
-        <v>110</v>
+        <v>184</v>
       </c>
       <c r="C33" s="7">
         <v>1</v>
@@ -1914,10 +1914,10 @@
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="H33" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1930,10 +1930,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>110</v>
+        <v>168</v>
+      </c>
+      <c r="B35" t="s">
+        <v>184</v>
       </c>
       <c r="C35" s="7">
         <v>1</v>
@@ -1942,10 +1942,10 @@
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="H35" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1956,7 +1956,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1970,10 +1970,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38" t="s">
         <v>183</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="C38" s="7">
         <v>1</v>
@@ -1982,72 +1982,72 @@
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="H38" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>110</v>
+        <v>172</v>
+      </c>
+      <c r="B39" t="s">
+        <v>183</v>
       </c>
       <c r="C39" s="7">
         <v>1</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="H39" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>110</v>
+        <v>173</v>
+      </c>
+      <c r="B40" t="s">
+        <v>183</v>
       </c>
       <c r="C40" s="7">
         <v>1</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="H40" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>110</v>
+        <v>174</v>
+      </c>
+      <c r="B41" t="s">
+        <v>183</v>
       </c>
       <c r="C41" s="7">
         <v>1</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="H41" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>16</v>
@@ -2058,10 +2058,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B45" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C45" t="b">
         <v>1</v>
@@ -2069,10 +2069,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B46" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C46" t="b">
         <v>1</v>
@@ -2080,10 +2080,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B47" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C47" t="b">
         <v>1</v>
@@ -2091,10 +2091,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B48" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C48" t="b">
         <v>1</v>
@@ -2102,10 +2102,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B49" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="C49" t="b">
         <v>1</v>
@@ -2113,10 +2113,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B50" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="C50" t="b">
         <v>1</v>
@@ -2124,10 +2124,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B51" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C51" t="b">
         <v>1</v>
@@ -2135,10 +2135,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B52" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C52" t="b">
         <v>1</v>
@@ -2146,10 +2146,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B53" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C53" t="b">
         <v>1</v>
@@ -2157,40 +2157,43 @@
     </row>
     <row r="55" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2202,8 +2205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FA9935-1338-5743-9994-8B53C9940146}">
   <dimension ref="A3:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="150" zoomScaleNormal="164" workbookViewId="0">
-      <selection activeCell="H85" sqref="H85"/>
+    <sheetView topLeftCell="A43" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2212,12 +2215,12 @@
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="21.1640625" customWidth="1"/>
     <col min="8" max="8" width="27.1640625" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" customWidth="1"/>
     <col min="11" max="11" width="6.33203125" customWidth="1"/>
     <col min="12" max="12" width="21.33203125" customWidth="1"/>
     <col min="13" max="13" width="24.33203125" customWidth="1"/>
@@ -2231,7 +2234,7 @@
     </row>
     <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>28</v>
@@ -2246,21 +2249,21 @@
         <v>39</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2268,7 +2271,7 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2276,7 +2279,7 @@
         <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2284,15 +2287,15 @@
         <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D9" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2300,7 +2303,7 @@
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2308,7 +2311,7 @@
         <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2324,21 +2327,21 @@
         <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
         <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2346,7 +2349,7 @@
         <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2354,21 +2357,21 @@
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
         <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2376,7 +2379,7 @@
         <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2384,21 +2387,21 @@
         <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
         <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -2406,7 +2409,7 @@
         <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2414,21 +2417,21 @@
         <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
         <v>33</v>
       </c>
       <c r="D27" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2436,7 +2439,7 @@
         <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -2444,7 +2447,7 @@
         <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2454,10 +2457,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>35</v>
@@ -2471,50 +2474,50 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" t="s">
         <v>96</v>
       </c>
-      <c r="B33" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" t="s">
-        <v>97</v>
-      </c>
-      <c r="D33" t="s">
-        <v>98</v>
-      </c>
       <c r="E33" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
         <v>96</v>
       </c>
-      <c r="B34" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" t="s">
-        <v>98</v>
-      </c>
       <c r="D34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" t="s">
         <v>99</v>
-      </c>
-      <c r="E34" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D35" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E35" t="s">
         <v>20</v>
@@ -2522,67 +2525,67 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C36" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D36" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E36" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E37" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
         <v>26</v>
       </c>
       <c r="E38" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
         <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E39" t="s">
         <v>32</v>
@@ -2590,50 +2593,50 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D41" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E41" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B42" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C42" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D42" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E42" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B43" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C43" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D43" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
@@ -2641,67 +2644,67 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C44" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D44" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E44" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E46" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B47" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C47" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D47" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B48" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C48" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D48" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E48" t="s">
         <v>20</v>
@@ -2709,67 +2712,67 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D49" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E49" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D51" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E51" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B52" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C52" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D52" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E52" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B53" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C53" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D53" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E53" t="s">
         <v>20</v>
@@ -2777,67 +2780,67 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C54" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D54" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E54" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C56" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E56" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B57" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C57" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D57" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E57" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B58" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C58" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D58" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E58" t="s">
         <v>20</v>
@@ -2845,19 +2848,19 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B59" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C59" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D59" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E59" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
@@ -2867,75 +2870,73 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E62" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="E62" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="F62" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J62" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G62" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="K62" s="1" t="s">
-        <v>131</v>
+      <c r="K62" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M62" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="N62" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="M62" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="N62" s="14"/>
     </row>
     <row r="64" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D64" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>136</v>
-      </c>
       <c r="E64" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="J64" s="4" t="s">
         <v>6</v>
@@ -2943,28 +2944,28 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="I66" s="4" t="s">
         <v>6</v>
@@ -2975,13 +2976,13 @@
         <v>30</v>
       </c>
       <c r="B67" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" t="s">
         <v>96</v>
       </c>
-      <c r="C67" t="s">
-        <v>98</v>
-      </c>
       <c r="D67" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E67" t="s">
         <v>31</v>
@@ -2995,16 +2996,16 @@
         <v>30</v>
       </c>
       <c r="B68" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C68" t="s">
         <v>26</v>
       </c>
       <c r="D68" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E68" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F68" t="b">
         <v>0</v>
@@ -3012,13 +3013,13 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>40</v>
@@ -3027,10 +3028,10 @@
         <v>41</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>42</v>
@@ -3041,19 +3042,20 @@
       <c r="J71" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="K71" s="4"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>31</v>
       </c>
       <c r="B72" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C72" t="s">
-        <v>97</v>
-      </c>
-      <c r="D72" t="s">
-        <v>172</v>
+        <v>95</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>180</v>
       </c>
       <c r="E72">
         <v>1500</v>
@@ -3064,8 +3066,8 @@
       <c r="G72">
         <v>10</v>
       </c>
-      <c r="H72" t="s">
-        <v>190</v>
+      <c r="H72" s="12" t="s">
+        <v>179</v>
       </c>
       <c r="I72" t="b">
         <v>0</v>
@@ -3073,24 +3075,27 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G74" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H74" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3099,10 +3104,10 @@
         <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C75" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
@@ -3111,18 +3116,18 @@
         <v>32</v>
       </c>
       <c r="F75" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>44</v>
@@ -3137,10 +3142,10 @@
         <v>43</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>6</v>
@@ -3148,37 +3153,37 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D79" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D79" s="5" t="s">
-        <v>136</v>
-      </c>
       <c r="E79" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>47</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="K79" s="5" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="L79" s="4" t="s">
         <v>6</v>
@@ -3189,16 +3194,16 @@
         <v>33</v>
       </c>
       <c r="B80" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C80" t="s">
+        <v>97</v>
+      </c>
+      <c r="D80" t="s">
         <v>99</v>
       </c>
-      <c r="D80" t="s">
-        <v>101</v>
-      </c>
       <c r="E80" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F80" t="b">
         <v>0</v>
@@ -3209,16 +3214,16 @@
         <v>33</v>
       </c>
       <c r="B82" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C82" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D82" t="s">
         <v>20</v>
       </c>
-      <c r="E82" t="s">
-        <v>157</v>
+      <c r="E82" s="12" t="s">
+        <v>181</v>
       </c>
       <c r="F82" t="b">
         <v>0</v>
@@ -3229,16 +3234,16 @@
         <v>33</v>
       </c>
       <c r="B84" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C84" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D84" t="s">
-        <v>103</v>
-      </c>
-      <c r="E84" t="s">
-        <v>158</v>
+        <v>100</v>
+      </c>
+      <c r="E84" s="12" t="s">
+        <v>182</v>
       </c>
       <c r="F84" t="b">
         <v>0</v>
@@ -3249,16 +3254,16 @@
         <v>33</v>
       </c>
       <c r="B86" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C86" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D86" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E86" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F86" t="b">
         <v>0</v>
@@ -3269,16 +3274,16 @@
         <v>33</v>
       </c>
       <c r="B88" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C88" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D88" t="s">
-        <v>103</v>
-      </c>
-      <c r="E88" t="s">
-        <v>158</v>
+        <v>100</v>
+      </c>
+      <c r="E88" s="12" t="s">
+        <v>182</v>
       </c>
       <c r="F88" t="b">
         <v>0</v>
@@ -3289,16 +3294,16 @@
         <v>33</v>
       </c>
       <c r="B89" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D89" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E89" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F89" t="b">
         <v>0</v>
@@ -3309,16 +3314,16 @@
         <v>33</v>
       </c>
       <c r="B90" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D90" t="s">
         <v>20</v>
       </c>
-      <c r="E90" t="s">
-        <v>157</v>
+      <c r="E90" s="12" t="s">
+        <v>181</v>
       </c>
       <c r="F90" t="b">
         <v>0</v>
@@ -3329,16 +3334,16 @@
         <v>33</v>
       </c>
       <c r="B92" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C92" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D92" t="s">
-        <v>103</v>
-      </c>
-      <c r="E92" t="s">
-        <v>158</v>
+        <v>100</v>
+      </c>
+      <c r="E92" s="12" t="s">
+        <v>182</v>
       </c>
       <c r="F92" t="b">
         <v>0</v>
@@ -3349,16 +3354,16 @@
         <v>33</v>
       </c>
       <c r="B93" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D93" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E93" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F93" t="b">
         <v>0</v>
@@ -3369,16 +3374,16 @@
         <v>33</v>
       </c>
       <c r="B94" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D94" t="s">
         <v>20</v>
       </c>
-      <c r="E94" t="s">
-        <v>157</v>
+      <c r="E94" s="12" t="s">
+        <v>181</v>
       </c>
       <c r="F94" t="b">
         <v>0</v>
@@ -3389,16 +3394,16 @@
         <v>33</v>
       </c>
       <c r="B96" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C96" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D96" t="s">
-        <v>103</v>
-      </c>
-      <c r="E96" t="s">
-        <v>158</v>
+        <v>100</v>
+      </c>
+      <c r="E96" s="12" t="s">
+        <v>182</v>
       </c>
       <c r="F96" t="b">
         <v>0</v>
@@ -3409,16 +3414,16 @@
         <v>33</v>
       </c>
       <c r="B97" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D97" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E97" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F97" t="b">
         <v>0</v>
@@ -3429,16 +3434,16 @@
         <v>33</v>
       </c>
       <c r="B98" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D98" t="s">
         <v>20</v>
       </c>
-      <c r="E98" t="s">
-        <v>157</v>
+      <c r="E98" s="12" t="s">
+        <v>181</v>
       </c>
       <c r="F98" t="b">
         <v>0</v>
@@ -3449,16 +3454,16 @@
         <v>33</v>
       </c>
       <c r="B100" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C100" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D100" t="s">
-        <v>103</v>
-      </c>
-      <c r="E100" t="s">
-        <v>158</v>
+        <v>100</v>
+      </c>
+      <c r="E100" s="12" t="s">
+        <v>182</v>
       </c>
       <c r="F100" t="b">
         <v>0</v>
@@ -3469,16 +3474,16 @@
         <v>33</v>
       </c>
       <c r="B101" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D101" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E101" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F101" t="b">
         <v>0</v>
@@ -3489,16 +3494,16 @@
         <v>33</v>
       </c>
       <c r="B102" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D102" t="s">
         <v>20</v>
       </c>
-      <c r="E102" t="s">
-        <v>157</v>
+      <c r="E102" s="12" t="s">
+        <v>181</v>
       </c>
       <c r="F102" t="b">
         <v>0</v>
@@ -3506,34 +3511,34 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G104" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G104" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="H104" s="1" t="s">
         <v>43</v>
       </c>
       <c r="I104" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="J104" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="K104" s="4" t="s">
         <v>6</v>
@@ -3541,13 +3546,13 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B105" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C105" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D105" t="b">
         <v>1</v>
@@ -3555,32 +3560,32 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="109" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="110" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -3590,10 +3595,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E788907-EF7B-7245-8B51-85EEFFE3B34D}">
-  <dimension ref="A2:D45"/>
+  <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3605,12 +3610,12 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>48</v>
@@ -3624,10 +3629,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>184</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C4">
         <v>128</v>
@@ -3638,10 +3643,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>184</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C5">
         <v>128</v>
@@ -3652,10 +3657,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C6">
         <v>1500</v>
@@ -3666,10 +3671,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" t="s">
         <v>110</v>
-      </c>
-      <c r="B7" t="s">
-        <v>114</v>
       </c>
       <c r="C7">
         <v>1500</v>
@@ -3680,10 +3685,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>184</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C8">
         <v>1000</v>
@@ -3694,10 +3699,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" t="s">
         <v>110</v>
-      </c>
-      <c r="B9" t="s">
-        <v>114</v>
       </c>
       <c r="C9">
         <v>1000</v>
@@ -3708,384 +3713,501 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>184</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C10">
         <v>1000</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>32.294883999999996</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>184</v>
       </c>
       <c r="B11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C11">
         <v>1000</v>
       </c>
       <c r="D11">
-        <v>32.294883999999996</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12">
-        <v>1000</v>
-      </c>
-      <c r="D12">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>183</v>
       </c>
       <c r="B13" t="s">
-        <v>191</v>
+        <v>106</v>
       </c>
       <c r="C13">
-        <v>1000</v>
+        <v>128</v>
       </c>
       <c r="D13">
-        <v>1000</v>
+        <f>2.33*D4</f>
+        <v>2.035221215</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>183</v>
       </c>
       <c r="B14" t="s">
-        <v>192</v>
+        <v>107</v>
       </c>
       <c r="C14">
-        <v>1000</v>
+        <v>128</v>
       </c>
       <c r="D14">
-        <v>500</v>
+        <f t="shared" ref="D14:D19" si="0">2.33*D5</f>
+        <v>1.458096525</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>110</v>
+        <v>183</v>
       </c>
       <c r="B15" t="s">
-        <v>193</v>
+        <v>109</v>
       </c>
       <c r="C15">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="D15">
-        <v>250</v>
+        <f t="shared" si="0"/>
+        <v>12.747525530000001</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16" t="s">
         <v>110</v>
       </c>
-      <c r="B16" t="s">
-        <v>194</v>
-      </c>
       <c r="C16">
+        <v>1500</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>10.615249329999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17">
         <v>1000</v>
       </c>
-      <c r="D16">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>8.8371168200000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18">
+        <v>1000</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>7.2162383400000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19">
+        <v>1000</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>75.247079719999988</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>145</v>
-      </c>
-      <c r="B20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24">
         <v>128</v>
       </c>
-      <c r="D20">
+      <c r="D24">
         <f>D4/5</f>
         <v>0.17469709999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>145</v>
-      </c>
-      <c r="B21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C21">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25">
         <v>128</v>
       </c>
-      <c r="D21">
-        <f t="shared" ref="D21:D25" si="0">D5/5</f>
+      <c r="D25">
+        <f t="shared" ref="D25:D29" si="1">D5/5</f>
         <v>0.12515850000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>145</v>
-      </c>
-      <c r="B22" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26">
         <v>1500</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
+      <c r="D26">
+        <f t="shared" si="1"/>
         <v>1.0942082000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>145</v>
-      </c>
-      <c r="B23" t="s">
-        <v>114</v>
-      </c>
-      <c r="C23">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27">
         <v>1500</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
+      <c r="D27">
+        <f t="shared" si="1"/>
         <v>0.91118019999999988</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>145</v>
-      </c>
-      <c r="B24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C24">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28">
         <v>1000</v>
       </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
+      <c r="D28">
+        <f t="shared" si="1"/>
         <v>0.75855079999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>145</v>
-      </c>
-      <c r="B25" t="s">
-        <v>114</v>
-      </c>
-      <c r="C25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29">
         <v>1000</v>
       </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
+      <c r="D29">
+        <f t="shared" si="1"/>
         <v>0.61941959999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>181</v>
-      </c>
-      <c r="B29" t="s">
-        <v>182</v>
-      </c>
-      <c r="C29">
-        <v>50</v>
-      </c>
-      <c r="D29">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F32" s="13"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>185</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>170</v>
       </c>
       <c r="C33">
-        <v>25.468708882538891</v>
+        <v>128</v>
       </c>
       <c r="D33">
-        <v>2.0314564440981862E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="E33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>185</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>170</v>
       </c>
       <c r="C34">
-        <v>26.615850225217656</v>
+        <v>1500</v>
       </c>
       <c r="D34">
-        <v>1.5806828571358057E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>118</v>
-      </c>
-      <c r="B35" t="s">
-        <v>116</v>
-      </c>
-      <c r="C35">
-        <v>26.33975299412786</v>
-      </c>
-      <c r="D35">
-        <v>1.6032781107754593E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" t="s">
-        <v>116</v>
-      </c>
-      <c r="C36">
-        <v>22.973998649851932</v>
-      </c>
-      <c r="D36">
-        <v>2.6475916111960041E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>119</v>
-      </c>
-      <c r="B37" t="s">
-        <v>116</v>
-      </c>
-      <c r="C37">
-        <v>23.006837790126468</v>
-      </c>
-      <c r="D37">
-        <v>2.3799811941421119E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="E34">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>117</v>
+        <v>188</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C38">
-        <v>27.641803043648572</v>
+        <v>128</v>
       </c>
       <c r="D38">
-        <v>2.0314564440981862E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24.56</v>
+      </c>
+      <c r="E38">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>118</v>
+        <v>188</v>
       </c>
       <c r="B39" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C39">
-        <v>28.105751672196035</v>
+        <v>512</v>
       </c>
       <c r="D39">
-        <v>1.7621004694522425E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+        <v>39.1</v>
+      </c>
+      <c r="E39">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>188</v>
+      </c>
+      <c r="B40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40">
+        <v>1500</v>
+      </c>
+      <c r="D40">
+        <v>55.85</v>
+      </c>
+      <c r="E40">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>186</v>
+      </c>
+      <c r="B42" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42">
+        <v>128</v>
+      </c>
+      <c r="D42">
+        <v>27.96</v>
+      </c>
+      <c r="E42">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>186</v>
+      </c>
+      <c r="B43" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43">
+        <v>512</v>
+      </c>
+      <c r="D43">
+        <v>29.12</v>
+      </c>
+      <c r="E43">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>186</v>
+      </c>
+      <c r="B44" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44">
+        <v>1500</v>
+      </c>
+      <c r="D44">
+        <v>30.210999999999999</v>
+      </c>
+      <c r="E44">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46">
+        <v>128</v>
+      </c>
+      <c r="D46">
+        <v>29.81</v>
+      </c>
+      <c r="E46">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47">
+        <v>512</v>
+      </c>
+      <c r="D47">
+        <v>39.21</v>
+      </c>
+      <c r="E47">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48">
+        <v>1500</v>
+      </c>
+      <c r="D48">
+        <v>50.22</v>
+      </c>
+      <c r="E48">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -4097,7 +4219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CD1F53-6FA9-024B-AEB4-78F83AE23C0B}">
   <dimension ref="A3:D35"/>
   <sheetViews>
-    <sheetView zoomScale="98" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -4117,7 +4239,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>22</v>
@@ -4131,13 +4253,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -4145,13 +4267,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" t="s">
         <v>96</v>
       </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -4159,13 +4281,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -4173,13 +4295,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C8" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -4187,13 +4309,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C9" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -4201,13 +4323,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -4215,13 +4337,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -4229,13 +4351,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -4243,13 +4365,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -4257,13 +4379,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C15" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -4271,13 +4393,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B16" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C16" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -4285,13 +4407,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C17" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="D17">
         <v>10</v>
@@ -4299,13 +4421,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C19" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D19">
         <v>10</v>
@@ -4313,13 +4435,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C20" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -4327,13 +4449,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B21" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C21" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D21">
         <v>10</v>
@@ -4341,13 +4463,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B23" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C23" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="D23">
         <v>10</v>
@@ -4355,13 +4477,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B24" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C24" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="D24">
         <v>10</v>
@@ -4369,13 +4491,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B25" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C25" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="D25">
         <v>10</v>
@@ -4383,13 +4505,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C27" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="D27">
         <v>10</v>
@@ -4397,13 +4519,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B28" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C28" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -4411,13 +4533,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B29" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C29" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="D29">
         <v>10</v>
@@ -4425,27 +4547,27 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -4455,10 +4577,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04436424-07DF-B343-BAAE-706A3CFD4756}">
-  <dimension ref="A2:K24"/>
+  <dimension ref="A2:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4467,44 +4589,44 @@
     <col min="3" max="3" width="7.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.5" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="13.83203125" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" customWidth="1"/>
+    <col min="10" max="10" width="9.5" customWidth="1"/>
     <col min="11" max="11" width="7" customWidth="1"/>
     <col min="12" max="12" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>43</v>
@@ -4512,7 +4634,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -4529,7 +4651,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="F5">
         <v>30</v>
@@ -4546,21 +4668,21 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>9</v>
@@ -4571,21 +4693,21 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>9</v>
@@ -4596,72 +4718,76 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" s="14"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F18" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="H18">
         <v>5</v>
@@ -4673,9 +4799,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F19" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="H19">
         <v>20</v>
@@ -4687,29 +4813,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -4721,8 +4847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0BE0C2-6CFA-B544-AD1B-E0CD7C820A66}">
   <dimension ref="A2:D11"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D11"/>
+    <sheetView tabSelected="1" zoomScale="251" zoomScaleNormal="251" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4732,133 +4858,133 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D3" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C4">
         <v>128</v>
       </c>
       <c r="D4">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C5">
         <v>256</v>
       </c>
       <c r="D5">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C6">
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="D6">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C7">
-        <v>256</v>
+        <v>1024</v>
       </c>
       <c r="D7">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C8">
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="D8">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C9">
-        <v>1024</v>
+        <v>256</v>
       </c>
       <c r="D9">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C10">
         <v>512</v>
       </c>
       <c r="D10">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C11">
         <v>1024</v>
       </c>
       <c r="D11">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>